<commit_message>
* set the locale to store * you can controlle languages over components
</commit_message>
<xml_diff>
--- a/meta/components/MenuBar.xlsx
+++ b/meta/components/MenuBar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaino/Desktop/dapanda-front-core/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA15933-A7EA-994A-947D-5850B93387CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFF6EB1-325E-9F40-B288-99BF93D2D547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1880" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="500" windowWidth="25200" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t>パッケージ</t>
   </si>
@@ -850,6 +850,14 @@
   </si>
   <si>
     <t>import NodeMenuItem from "%/components/menu/NodeMenuItem/NodeMenuItem.vue"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>LocaleSelect</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import LocaleSelect from "%/components/LocaleSelect/LocaleSelect.vue"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1661,6 +1669,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1669,45 +1716,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2120,10 +2128,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2238,10 +2246,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="102"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="10"/>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2253,10 +2261,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="102"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="10"/>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2268,10 +2276,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2285,10 +2293,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2306,11 +2314,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2449,10 +2457,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2479,10 +2487,10 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="107"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
@@ -2496,10 +2504,10 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="107"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
@@ -2600,8 +2608,12 @@
       <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="52"/>
-      <c r="B32" s="48"/>
+      <c r="A32" s="52">
+        <v>3</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>94</v>
+      </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
       <c r="E32" s="50"/>
@@ -2615,84 +2627,80 @@
       <c r="M32" s="35"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="35"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="44" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="47" t="s">
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="51">
-        <v>1</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
       <c r="M36" s="35"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
+        <v>89</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
       <c r="F37" s="68"/>
       <c r="G37" s="68"/>
       <c r="H37" s="68"/>
@@ -2703,11 +2711,15 @@
       <c r="M37" s="35"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="52"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
+      <c r="A38" s="51">
+        <v>2</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
       <c r="H38" s="68"/>
@@ -2718,11 +2730,15 @@
       <c r="M38" s="35"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="83"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
+      <c r="A39" s="52">
+        <v>3</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
       <c r="H39" s="68"/>
@@ -2733,79 +2749,79 @@
       <c r="M39" s="35"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="35"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="83"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="35"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="44" t="s">
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="47" t="s">
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B43" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="51"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="51"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="45"/>
       <c r="M43" s="35"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="52"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="50"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="39"/>
       <c r="F44" s="68"/>
       <c r="G44" s="68"/>
       <c r="H44" s="68"/>
@@ -2816,95 +2832,95 @@
       <c r="M44" s="35"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="35"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="52"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="35"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="44" t="s">
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="47" t="s">
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B49" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="C49" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D49" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="82"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="51"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="87"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="51"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="45"/>
       <c r="M49" s="35"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="52"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="50"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="39"/>
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
       <c r="H50" s="68"/>
@@ -2915,11 +2931,11 @@
       <c r="M50" s="35"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="83"/>
-      <c r="B51" s="84"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
+      <c r="A51" s="51"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="41"/>
       <c r="F51" s="68"/>
       <c r="G51" s="68"/>
       <c r="H51" s="68"/>
@@ -2930,81 +2946,81 @@
       <c r="M51" s="35"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="52"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="35"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="83"/>
+      <c r="B53" s="84"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="68"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="35"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="44" t="s">
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="47" t="s">
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="43"/>
+      <c r="M54" s="43"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B55" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="67" t="s">
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="82"/>
+      <c r="F55" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="45"/>
-      <c r="L53" s="45"/>
-      <c r="M53" s="35"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="51"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
-      <c r="M54" s="35"/>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="51"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
+      <c r="G55" s="67"/>
+      <c r="H55" s="67"/>
+      <c r="I55" s="67"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="45"/>
       <c r="M55" s="35"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="52"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="50"/>
+      <c r="A56" s="51"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="39"/>
       <c r="F56" s="68"/>
       <c r="G56" s="68"/>
       <c r="H56" s="68"/>
@@ -3015,138 +3031,132 @@
       <c r="M56" s="35"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="A57" s="51"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="35"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13" t="s">
+      <c r="A58" s="52"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="68"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="36"/>
+      <c r="K58" s="36"/>
+      <c r="L58" s="36"/>
+      <c r="M58" s="35"/>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="13"/>
+      <c r="B60" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="3" t="s">
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="15"/>
-    </row>
-    <row r="60" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A60" s="100" t="s">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="15"/>
+    </row>
+    <row r="62" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A62" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="100" t="s">
+      <c r="B62" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="97" t="s">
+      <c r="C62" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="97" t="s">
+      <c r="D62" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="97" t="s">
+      <c r="E62" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="98" t="s">
+      <c r="F62" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="98" t="s">
+      <c r="G62" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="108" t="s">
+      <c r="H62" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="97" t="s">
+      <c r="I62" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="J60" s="97"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="9"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="100"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="99"/>
-      <c r="G61" s="99"/>
-      <c r="H61" s="109"/>
-      <c r="I61" s="97"/>
-      <c r="J61" s="97"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="15"/>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62" s="19">
-        <v>1</v>
-      </c>
-      <c r="B62" s="71"/>
-      <c r="C62" s="78"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="69"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="28"/>
-      <c r="M62" s="15"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="9"/>
     </row>
     <row r="63" spans="1:13">
-      <c r="A63" s="19">
-        <f>A62+1</f>
-        <v>2</v>
-      </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="69"/>
-      <c r="H63" s="69"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="28"/>
+      <c r="A63" s="97"/>
+      <c r="B63" s="97"/>
+      <c r="C63" s="96"/>
+      <c r="D63" s="96"/>
+      <c r="E63" s="96"/>
+      <c r="F63" s="101"/>
+      <c r="G63" s="101"/>
+      <c r="H63" s="99"/>
+      <c r="I63" s="96"/>
+      <c r="J63" s="96"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="29"/>
       <c r="M63" s="15"/>
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="19">
-        <f t="shared" ref="A64:A78" si="0">A63+1</f>
-        <v>3</v>
-      </c>
-      <c r="B64" s="72"/>
-      <c r="C64" s="79"/>
+        <v>1</v>
+      </c>
+      <c r="B64" s="71"/>
+      <c r="C64" s="78"/>
       <c r="D64" s="20"/>
       <c r="E64" s="20"/>
       <c r="F64" s="20"/>
@@ -3155,16 +3165,16 @@
       <c r="I64" s="20"/>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
-      <c r="L64" s="22"/>
+      <c r="L64" s="28"/>
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="80"/>
+        <f>A64+1</f>
+        <v>2</v>
+      </c>
+      <c r="B65" s="71"/>
+      <c r="C65" s="78"/>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
       <c r="F65" s="20"/>
@@ -3173,16 +3183,16 @@
       <c r="I65" s="20"/>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
-      <c r="L65" s="22"/>
+      <c r="L65" s="28"/>
       <c r="M65" s="15"/>
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
+        <f t="shared" ref="A66:A80" si="0">A65+1</f>
+        <v>3</v>
+      </c>
+      <c r="B66" s="72"/>
+      <c r="C66" s="79"/>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
@@ -3197,25 +3207,25 @@
     <row r="67" spans="1:13">
       <c r="A67" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B67" s="73"/>
       <c r="C67" s="80"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="76"/>
-      <c r="K67" s="76"/>
-      <c r="L67" s="77"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="69"/>
+      <c r="H67" s="69"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
       <c r="M67" s="15"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B68" s="73"/>
       <c r="C68" s="80"/>
@@ -3233,7 +3243,7 @@
     <row r="69" spans="1:13">
       <c r="A69" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B69" s="73"/>
       <c r="C69" s="80"/>
@@ -3251,43 +3261,43 @@
     <row r="70" spans="1:13">
       <c r="A70" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B70" s="73"/>
       <c r="C70" s="80"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="76"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="77"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="69"/>
+      <c r="H70" s="69"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="22"/>
       <c r="M70" s="15"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B71" s="73"/>
       <c r="C71" s="80"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="69"/>
-      <c r="H71" s="69"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="22"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="75"/>
+      <c r="H71" s="75"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="76"/>
+      <c r="L71" s="77"/>
       <c r="M71" s="15"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B72" s="73"/>
       <c r="C72" s="80"/>
@@ -3305,43 +3315,43 @@
     <row r="73" spans="1:13">
       <c r="A73" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B73" s="73"/>
       <c r="C73" s="80"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-      <c r="F73" s="74"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="74"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="76"/>
-      <c r="L73" s="77"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="22"/>
       <c r="M73" s="15"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B74" s="73"/>
       <c r="C74" s="80"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="69"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="22"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="74"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="77"/>
       <c r="M74" s="15"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B75" s="73"/>
       <c r="C75" s="80"/>
@@ -3359,43 +3369,43 @@
     <row r="76" spans="1:13">
       <c r="A76" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B76" s="73"/>
       <c r="C76" s="80"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="74"/>
-      <c r="J76" s="76"/>
-      <c r="K76" s="76"/>
-      <c r="L76" s="77"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="69"/>
+      <c r="H76" s="69"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="22"/>
       <c r="M76" s="15"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B77" s="73"/>
       <c r="C77" s="80"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="69"/>
-      <c r="I77" s="20"/>
-      <c r="J77" s="21"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="22"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="74"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="76"/>
+      <c r="L77" s="77"/>
       <c r="M77" s="15"/>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B78" s="73"/>
       <c r="C78" s="80"/>
@@ -3411,94 +3421,100 @@
       <c r="M78" s="15"/>
     </row>
     <row r="79" spans="1:13">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="70"/>
-      <c r="H79" s="70"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="26"/>
-      <c r="L79" s="27"/>
+      <c r="A79" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="69"/>
+      <c r="H79" s="69"/>
+      <c r="I79" s="20"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="22"/>
       <c r="M79" s="15"/>
     </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B80" s="73"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="75"/>
+      <c r="H80" s="75"/>
+      <c r="I80" s="74"/>
+      <c r="J80" s="76"/>
+      <c r="K80" s="76"/>
+      <c r="L80" s="77"/>
+      <c r="M80" s="15"/>
+    </row>
     <row r="81" spans="1:13">
-      <c r="A81" s="30" t="s">
+      <c r="A81" s="23"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="70"/>
+      <c r="H81" s="70"/>
+      <c r="I81" s="25"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="27"/>
+      <c r="M81" s="15"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="31"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="81"/>
-      <c r="F81" s="44" t="s">
+      <c r="B83" s="31"/>
+      <c r="C83" s="31"/>
+      <c r="D83" s="31"/>
+      <c r="E83" s="81"/>
+      <c r="F83" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="43"/>
-      <c r="K81" s="43"/>
-      <c r="L81" s="43"/>
-      <c r="M81" s="43"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="47" t="s">
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="43"/>
+      <c r="L83" s="43"/>
+      <c r="M83" s="43"/>
+    </row>
+    <row r="84" spans="1:13">
+      <c r="A84" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="42" t="s">
+      <c r="B84" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="42"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="82"/>
-      <c r="F82" s="67"/>
-      <c r="G82" s="67"/>
-      <c r="H82" s="67"/>
-      <c r="I82" s="67"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="45"/>
-      <c r="L82" s="45"/>
-      <c r="M82" s="35"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="51"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
-      <c r="L83" s="36"/>
-      <c r="M83" s="35"/>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84" s="51"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="41"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="36"/>
-      <c r="K84" s="36"/>
-      <c r="L84" s="36"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="82"/>
+      <c r="F84" s="67"/>
+      <c r="G84" s="67"/>
+      <c r="H84" s="67"/>
+      <c r="I84" s="67"/>
+      <c r="J84" s="44"/>
+      <c r="K84" s="45"/>
+      <c r="L84" s="45"/>
       <c r="M84" s="35"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="52"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="49"/>
-      <c r="D85" s="49"/>
-      <c r="E85" s="50"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="39"/>
       <c r="F85" s="68"/>
       <c r="G85" s="68"/>
       <c r="H85" s="68"/>
@@ -3509,130 +3525,124 @@
       <c r="M85" s="35"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
+      <c r="A86" s="51"/>
+      <c r="B86" s="46"/>
+      <c r="C86" s="40"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="41"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="68"/>
+      <c r="H86" s="68"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="36"/>
+      <c r="M86" s="35"/>
     </row>
     <row r="87" spans="1:13">
-      <c r="A87" s="13"/>
-      <c r="B87" s="13" t="s">
+      <c r="A87" s="52"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="49"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="68"/>
+      <c r="I87" s="34"/>
+      <c r="J87" s="36"/>
+      <c r="K87" s="36"/>
+      <c r="L87" s="36"/>
+      <c r="M87" s="35"/>
+    </row>
+    <row r="88" spans="1:13">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88" s="3" t="s">
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="14"/>
-      <c r="L88" s="6"/>
-      <c r="M88" s="15"/>
-    </row>
-    <row r="89" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A89" s="100" t="s">
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="15"/>
+    </row>
+    <row r="91" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A91" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="100" t="s">
+      <c r="B91" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="C89" s="97" t="s">
+      <c r="C91" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="D89" s="97" t="s">
+      <c r="D91" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E89" s="97" t="s">
+      <c r="E91" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="F89" s="94"/>
-      <c r="G89" s="94"/>
-      <c r="H89" s="94"/>
-      <c r="I89" s="96"/>
-      <c r="J89" s="97"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="17"/>
-      <c r="M89" s="9"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="100"/>
-      <c r="B90" s="100"/>
-      <c r="C90" s="97"/>
-      <c r="D90" s="97"/>
-      <c r="E90" s="97"/>
-      <c r="F90" s="95"/>
-      <c r="G90" s="95"/>
-      <c r="H90" s="95"/>
-      <c r="I90" s="96"/>
-      <c r="J90" s="97"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="15"/>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91" s="19">
-        <v>1</v>
-      </c>
-      <c r="B91" s="71"/>
-      <c r="C91" s="78"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="90"/>
-      <c r="G91" s="92"/>
-      <c r="H91" s="92"/>
-      <c r="I91" s="90"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
-      <c r="L91" s="28"/>
-      <c r="M91" s="15"/>
+      <c r="F91" s="107"/>
+      <c r="G91" s="107"/>
+      <c r="H91" s="107"/>
+      <c r="I91" s="109"/>
+      <c r="J91" s="96"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="17"/>
+      <c r="M91" s="9"/>
     </row>
     <row r="92" spans="1:13">
-      <c r="A92" s="19">
-        <f>A91+1</f>
-        <v>2</v>
-      </c>
-      <c r="B92" s="71"/>
-      <c r="C92" s="78"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="90"/>
-      <c r="G92" s="92"/>
-      <c r="H92" s="92"/>
-      <c r="I92" s="90"/>
-      <c r="J92" s="21"/>
-      <c r="K92" s="21"/>
-      <c r="L92" s="28"/>
+      <c r="A92" s="97"/>
+      <c r="B92" s="97"/>
+      <c r="C92" s="96"/>
+      <c r="D92" s="96"/>
+      <c r="E92" s="96"/>
+      <c r="F92" s="108"/>
+      <c r="G92" s="108"/>
+      <c r="H92" s="108"/>
+      <c r="I92" s="109"/>
+      <c r="J92" s="96"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="29"/>
       <c r="M92" s="15"/>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="19">
-        <f t="shared" ref="A93:A97" si="1">A92+1</f>
-        <v>3</v>
-      </c>
-      <c r="B93" s="72"/>
-      <c r="C93" s="79"/>
+        <v>1</v>
+      </c>
+      <c r="B93" s="71"/>
+      <c r="C93" s="78"/>
       <c r="D93" s="20"/>
       <c r="E93" s="20"/>
       <c r="F93" s="90"/>
@@ -3641,16 +3651,16 @@
       <c r="I93" s="90"/>
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
-      <c r="L93" s="22"/>
+      <c r="L93" s="28"/>
       <c r="M93" s="15"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B94" s="73"/>
-      <c r="C94" s="80"/>
+        <f>A93+1</f>
+        <v>2</v>
+      </c>
+      <c r="B94" s="71"/>
+      <c r="C94" s="78"/>
       <c r="D94" s="20"/>
       <c r="E94" s="20"/>
       <c r="F94" s="90"/>
@@ -3659,16 +3669,16 @@
       <c r="I94" s="90"/>
       <c r="J94" s="21"/>
       <c r="K94" s="21"/>
-      <c r="L94" s="22"/>
+      <c r="L94" s="28"/>
       <c r="M94" s="15"/>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="19">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B95" s="73"/>
-      <c r="C95" s="80"/>
+        <f t="shared" ref="A95:A99" si="1">A94+1</f>
+        <v>3</v>
+      </c>
+      <c r="B95" s="72"/>
+      <c r="C95" s="79"/>
       <c r="D95" s="20"/>
       <c r="E95" s="20"/>
       <c r="F95" s="90"/>
@@ -3683,25 +3693,25 @@
     <row r="96" spans="1:13">
       <c r="A96" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B96" s="73"/>
       <c r="C96" s="80"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="91"/>
-      <c r="G96" s="93"/>
-      <c r="H96" s="93"/>
-      <c r="I96" s="91"/>
-      <c r="J96" s="76"/>
-      <c r="K96" s="76"/>
-      <c r="L96" s="77"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="90"/>
+      <c r="G96" s="92"/>
+      <c r="H96" s="92"/>
+      <c r="I96" s="90"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="22"/>
       <c r="M96" s="15"/>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="19">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B97" s="73"/>
       <c r="C97" s="80"/>
@@ -3716,38 +3726,74 @@
       <c r="L97" s="22"/>
       <c r="M97" s="15"/>
     </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B98" s="73"/>
+      <c r="C98" s="80"/>
+      <c r="D98" s="74"/>
+      <c r="E98" s="74"/>
+      <c r="F98" s="91"/>
+      <c r="G98" s="93"/>
+      <c r="H98" s="93"/>
+      <c r="I98" s="91"/>
+      <c r="J98" s="76"/>
+      <c r="K98" s="76"/>
+      <c r="L98" s="77"/>
+      <c r="M98" s="15"/>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B99" s="73"/>
+      <c r="C99" s="80"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="90"/>
+      <c r="G99" s="92"/>
+      <c r="H99" s="92"/>
+      <c r="I99" s="90"/>
+      <c r="J99" s="21"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I60:J61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="I91:J92"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:J90"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I62:J63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E101:H101" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E103:H103" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3757,7 +3803,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F62:G79 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F64:G81 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">

</xml_diff>